<commit_message>
Add the minimum year to train and check
Signed-off-by: Supun De Silva <supun1001@gmail.com>
</commit_message>
<xml_diff>
--- a/data_samples/afl_ground_names.xlsx
+++ b/data_samples/afl_ground_names.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\ML101\data_samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C367A2B8-F3BB-4E24-827E-6D6BA6BC6F3A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{237B07DA-2580-4D65-A57A-2FBF5FBB2190}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
   <si>
     <t>Telstra Dome</t>
   </si>
@@ -553,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25:G28"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -653,13 +653,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="G7">
         <v>6</v>
@@ -667,245 +664,223 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
       </c>
       <c r="G8">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G10">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="G11">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G12">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="G13">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>27</v>
+      </c>
+      <c r="C14" t="s">
+        <v>59</v>
       </c>
       <c r="G14">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="G15">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="G16">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="B17" t="s">
+        <v>32</v>
       </c>
       <c r="G17">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="G18">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B19" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="G19">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B20" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="G20">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B21" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G21">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B22" t="s">
-        <v>55</v>
+        <v>42</v>
+      </c>
+      <c r="C22" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" t="s">
+        <v>41</v>
       </c>
       <c r="G22">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="G23">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B24" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="C24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D24" t="s">
-        <v>41</v>
+        <v>47</v>
+      </c>
+      <c r="E24" t="s">
+        <v>48</v>
       </c>
       <c r="G24">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>44</v>
-      </c>
-      <c r="B25" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="G25">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>46</v>
-      </c>
-      <c r="B26" t="s">
-        <v>56</v>
-      </c>
-      <c r="C26" t="s">
-        <v>57</v>
-      </c>
-      <c r="D26" t="s">
-        <v>47</v>
-      </c>
-      <c r="E26" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G26">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>50</v>
-      </c>
-      <c r="G27">
         <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>51</v>
-      </c>
-      <c r="G28">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>